<commit_message>
made validate test names consistent
</commit_message>
<xml_diff>
--- a/Documents/Testing/TestsDocuments/BB+WB_validate.xlsx
+++ b/Documents/Testing/TestsDocuments/BB+WB_validate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10719"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/da3f1eef4c95e50f/Documents/sft/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cescadelacruz/Documents/GitHub/SUM23-SFT221-NAA-4/Documents/Testing/TestsDocuments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1CBAF213-1990-4691-B1BC-613812D5E750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE08B56C-A3CC-5B4A-BA82-0C504BECA1B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -89,21 +89,6 @@
     <t xml:space="preserve">Test Function: </t>
   </si>
   <si>
-    <t>BB_Testvalidate1</t>
-  </si>
-  <si>
-    <t>BB_Testvalidate6</t>
-  </si>
-  <si>
-    <t>BB_Testvalidate5</t>
-  </si>
-  <si>
-    <t>BB_Testvalidate4</t>
-  </si>
-  <si>
-    <t>BB_Testvalidate3</t>
-  </si>
-  <si>
     <t>Entering a valid input</t>
   </si>
   <si>
@@ -164,15 +149,6 @@
     <t>Blackbox and Whitebox</t>
   </si>
   <si>
-    <t>WB_Testvalidate1</t>
-  </si>
-  <si>
-    <t>WB_Testvalidate2</t>
-  </si>
-  <si>
-    <t>WB_Testvalidate3</t>
-  </si>
-  <si>
     <t>Weight = 500, volume =0.5, Point p1={3,-1}</t>
   </si>
   <si>
@@ -194,7 +170,32 @@
     <t>To ensure the function returns the valid entry whether it is the weight , volume or destination contained in the struct point.</t>
   </si>
   <si>
-    <t>1. Recognize the constraints and the requirements of the validate function.                                                                                                                                                                                                     2. Testing both valid and invalid test cases.                                                                                                                              3. Compareing the actual results to the predicted results.</t>
+    <t>1. Recognize the constraints and the requirements of the validate function.                                                                                                                                                                                                     2. Testing both valid and invalid test cases.                                                                                                                            
+ 3. Compareing the actual results to the predicted results.</t>
+  </si>
+  <si>
+    <t>WB_validate1</t>
+  </si>
+  <si>
+    <t>WB_validate2</t>
+  </si>
+  <si>
+    <t>WB_validate3</t>
+  </si>
+  <si>
+    <t>BB_validate1</t>
+  </si>
+  <si>
+    <t>BB_validate3</t>
+  </si>
+  <si>
+    <t>BB_validate4</t>
+  </si>
+  <si>
+    <t>BB_validate5</t>
+  </si>
+  <si>
+    <t>BB_validate6</t>
   </si>
 </sst>
 </file>
@@ -403,6 +404,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -424,6 +428,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -436,6 +446,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -444,21 +460,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -742,144 +743,144 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="10"/>
-    </row>
-    <row r="3" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A3" s="11" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="11"/>
+    </row>
+    <row r="3" spans="1:9" ht="24" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="13"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="14"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="18">
         <v>4</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="16"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="19"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="18"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="21"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="18"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="21"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="18"/>
-    </row>
-    <row r="9" spans="1:9" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="21"/>
+    </row>
+    <row r="9" spans="1:9" ht="48.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="26"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="23"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="18"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="21"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="76.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="24"/>
+    <row r="12" spans="1:9" ht="76.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -902,30 +903,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B529C7-E270-4893-96A7-E1315BD69EEA}">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.21875" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.1640625" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" customWidth="1"/>
     <col min="3" max="3" width="65.33203125" customWidth="1"/>
-    <col min="4" max="4" width="37.5546875" customWidth="1"/>
-    <col min="5" max="5" width="56.109375" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="37.5" customWidth="1"/>
+    <col min="5" max="5" width="56.1640625" customWidth="1"/>
+    <col min="6" max="6" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="21"/>
-    </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="26"/>
+    </row>
+    <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -942,217 +943,217 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="43.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="53.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="53.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="22" t="s">
-        <v>33</v>
+      <c r="C4" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="56.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="58.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="74.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="74.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E32" s="3"/>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E33" s="3"/>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E34" s="3"/>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E35" s="3"/>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E36" s="3"/>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E37" s="3"/>
     </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E38" s="3"/>
     </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E39" s="3"/>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E40" s="3"/>
     </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E41" s="3"/>
     </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E42" s="3"/>
     </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E43" s="3"/>
     </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E44" s="3"/>
     </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E45" s="3"/>
     </row>
   </sheetData>
@@ -1169,29 +1170,29 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" customWidth="1"/>
     <col min="3" max="3" width="65.33203125" customWidth="1"/>
-    <col min="4" max="4" width="16.88671875" customWidth="1"/>
-    <col min="5" max="5" width="56.109375" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" customWidth="1"/>
+    <col min="5" max="5" width="56.1640625" customWidth="1"/>
+    <col min="6" max="6" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="21"/>
-    </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="26"/>
+    </row>
+    <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1208,175 +1209,175 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="64.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="55.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>42</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="56.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>46</v>
-      </c>
-      <c r="D4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>43</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="1:5" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E32" s="3"/>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E33" s="3"/>
     </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E34" s="3"/>
     </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E35" s="3"/>
     </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E36" s="3"/>
     </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E37" s="3"/>
     </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E38" s="3"/>
     </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E39" s="3"/>
     </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E40" s="3"/>
     </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E41" s="3"/>
     </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E42" s="3"/>
     </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E43" s="3"/>
     </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E44" s="3"/>
     </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E45" s="3"/>
     </row>
   </sheetData>
@@ -1388,21 +1389,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008641478389A1824A98F5C5E0B6162E5F" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9ef4b42a3ed9448361827c423e89ef89">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="81b064ac-ebcb-49a1-93f6-e61f75bebfa7" xmlns:ns3="717d1b07-b5a1-4bb5-9d40-3a9b6c764643" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0bb8b9f62ca6562dff4b6b6c0721aa08" ns2:_="" ns3:_="">
     <xsd:import namespace="81b064ac-ebcb-49a1-93f6-e61f75bebfa7"/>
@@ -1573,32 +1559,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D20CED7A-A184-4DAD-98D0-D68B5D737C5B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="7db3b190-d1cf-4882-bee6-3064ce691739"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="7e7c8aa9-4be2-48a6-a0f7-80013db2e73b"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A445DA8-61DA-4B15-A75B-C715E0A15404}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35A5AAF0-BBBC-48E3-AADB-8E4922D37D7D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1615,4 +1591,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A445DA8-61DA-4B15-A75B-C715E0A15404}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D20CED7A-A184-4DAD-98D0-D68B5D737C5B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="7db3b190-d1cf-4882-bee6-3064ce691739"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="7e7c8aa9-4be2-48a6-a0f7-80013db2e73b"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated validate() function docs.
Function specification and test case description files have been updated
</commit_message>
<xml_diff>
--- a/Documents/Testing/TestsDocuments/BB+WB_validate.xlsx
+++ b/Documents/Testing/TestsDocuments/BB+WB_validate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irish\Documents\SUM23-SFT221-NAA-4\Documents\Testing\TestsDocuments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{509C8407-2F87-4134-B32B-4F2709C0AF1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CDA8A4-A665-4428-865D-7398B4E30DA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="60">
   <si>
     <t>SFT 221</t>
   </si>
@@ -118,9 +118,6 @@
     <t>INVALID_POINT</t>
   </si>
   <si>
-    <t>Weight = 500, volume =0.5, Point p1={3,2}</t>
-  </si>
-  <si>
     <t>Weight = 0, volume =0.5, Point p1={3,4}</t>
   </si>
   <si>
@@ -136,9 +133,6 @@
     <t>Weight = 1500, volume =1.5, Point p1={-1,-1}</t>
   </si>
   <si>
-    <t>Gulpreet Kaur</t>
-  </si>
-  <si>
     <t>validate</t>
   </si>
   <si>
@@ -166,57 +160,73 @@
     <t>To ensure the function returns the valid entry whether it is the weight , volume or destination contained in the struct point.</t>
   </si>
   <si>
+    <t>WB_validate1</t>
+  </si>
+  <si>
+    <t>WB_validate2</t>
+  </si>
+  <si>
+    <t>WB_validate3</t>
+  </si>
+  <si>
+    <t>BB_validate1</t>
+  </si>
+  <si>
+    <t>BB_validate3</t>
+  </si>
+  <si>
+    <t>BB_validate4</t>
+  </si>
+  <si>
+    <t>BB_validate5</t>
+  </si>
+  <si>
+    <t>BB_validate6</t>
+  </si>
+  <si>
+    <t>Pass/ Fail</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Pass/Fail</t>
+  </si>
+  <si>
+    <t>Expected Results</t>
+  </si>
+  <si>
+    <t>Actual Results</t>
+  </si>
+  <si>
+    <t>Matches expected result</t>
+  </si>
+  <si>
+    <t>Weight = 500, volume =0.5, Point p1={2,2}</t>
+  </si>
+  <si>
+    <t>Gulpreet Kaur, Irish Banga</t>
+  </si>
+  <si>
     <t>1. Recognize the constraints and the requirements of the validate function.                                                                                                                                                                                                     2. Testing both valid and invalid test cases.                                                                                                                            
- 3. Compareing the actual results to the predicted results.</t>
-  </si>
-  <si>
-    <t>WB_validate1</t>
-  </si>
-  <si>
-    <t>WB_validate2</t>
-  </si>
-  <si>
-    <t>WB_validate3</t>
-  </si>
-  <si>
-    <t>BB_validate1</t>
-  </si>
-  <si>
-    <t>BB_validate3</t>
-  </si>
-  <si>
-    <t>BB_validate4</t>
-  </si>
-  <si>
-    <t>BB_validate5</t>
-  </si>
-  <si>
-    <t>BB_validate6</t>
-  </si>
-  <si>
-    <t>Pass/ Fail</t>
-  </si>
-  <si>
-    <t>Pass</t>
-  </si>
-  <si>
-    <t>Pass/Fail</t>
-  </si>
-  <si>
-    <t>Expected Results</t>
-  </si>
-  <si>
-    <t>Actual Results</t>
-  </si>
-  <si>
-    <t>Matches expected result</t>
+ 3. Comparing the actual results to the predicted results.</t>
+  </si>
+  <si>
+    <t>BUGS ENCOUNTERED?</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>YES; The function allowed for non-building destinations. 
+The test values have been updated to match the updated functionality.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,8 +262,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -293,6 +310,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -421,13 +443,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -457,6 +480,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -520,13 +546,17 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
     <cellStyle name="60% - Accent3" xfId="2" builtinId="40"/>
+    <cellStyle name="Bad" xfId="4" builtinId="27"/>
     <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -808,8 +838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -818,116 +848,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="15"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="16"/>
     </row>
     <row r="3" spans="1:9" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="18"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="19"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="23">
         <v>4</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="24"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="25"/>
+      <c r="B6" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="26"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="25"/>
+      <c r="B7" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="26"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="25"/>
+      <c r="B8" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="26"/>
     </row>
     <row r="9" spans="1:9" ht="48.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="27"/>
+      <c r="B9" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="27"/>
+      <c r="I9" s="28"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="26"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
@@ -935,17 +965,17 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="76.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="21"/>
+      <c r="A12" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -966,10 +996,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29B529C7-E270-4893-96A7-E1315BD69EEA}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -981,20 +1011,21 @@
     <col min="5" max="5" width="37.44140625" customWidth="1"/>
     <col min="6" max="6" width="56.109375" customWidth="1"/>
     <col min="7" max="7" width="19.21875" customWidth="1"/>
+    <col min="8" max="8" width="33.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="30"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="31"/>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="1:7" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1008,18 +1039,21 @@
         <v>9</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="43.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+      <c r="H2" s="35" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -1028,21 +1062,24 @@
         <v>15</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="E3" t="s">
         <v>21</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G3" s="34" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="53.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="53.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -1051,21 +1088,24 @@
         <v>16</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
         <v>22</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="G4" s="34" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -1074,21 +1114,24 @@
         <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
         <v>23</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" s="34" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -1097,21 +1140,24 @@
         <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
         <v>25</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G6" s="34" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="58.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
@@ -1120,21 +1166,24 @@
         <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
         <v>25</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G7" s="34" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="74.55" customHeight="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="74.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
@@ -1143,40 +1192,43 @@
         <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
         <v>24</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8" s="34" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.3">
@@ -1277,10 +1329,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29DBEBE5-E65B-48FE-ACB2-E1CF3882866A}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView zoomScale="77" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G5"/>
+    <sheetView topLeftCell="D1" zoomScale="77" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1292,20 +1344,21 @@
     <col min="5" max="5" width="29.33203125" customWidth="1"/>
     <col min="6" max="6" width="56.109375" customWidth="1"/>
     <col min="7" max="7" width="19.6640625" customWidth="1"/>
+    <col min="8" max="8" width="31.21875" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="33"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="34"/>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="1:7" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1319,115 +1372,127 @@
         <v>9</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="H2" s="35" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G3" s="34" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E4" t="s">
         <v>22</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G4" s="34" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="56.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" s="34" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:7" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.3">

</xml_diff>